<commit_message>
positions from different expiries
</commit_message>
<xml_diff>
--- a/backtest results/strangle backtests/BNF rollin strangle.xlsx
+++ b/backtest results/strangle backtests/BNF rollin strangle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aniket.bhadane/Desktop/General/AniketBhadane.github.io/backtest results/strangle backtests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE2E3D5-17F6-0845-846F-30C8251D2317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33637820-0DA6-C747-A4CF-3CD0AF9DA083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{0BAA9281-11C9-BF4F-A98E-3F6D4B70F5CF}"/>
   </bookViews>
@@ -7780,7 +7780,7 @@
   <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>